<commit_message>
Update MPPT code and Beacon testing data
</commit_message>
<xml_diff>
--- a/Power/Measurements.xlsx
+++ b/Power/Measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\YEAR 2\PROJECT\power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9C6C57-F6A4-4CF0-BA08-61C954B69819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EFC976-002B-4419-A6CF-441593E14464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="5580" windowWidth="23085" windowHeight="10485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
   <si>
     <t>V</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t xml:space="preserve">RELATIVE SUNNY </t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>BLUE</t>
   </si>
 </sst>
 </file>
@@ -6027,6 +6039,1056 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>I-V</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> Curve of Beacons</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15461731955307439"/>
+          <c:y val="0.12153297682709449"/>
+          <c:w val="0.74780798072408017"/>
+          <c:h val="0.63460496582312242"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>YELLOW</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AF$3:$AF$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.71</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.72</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.84</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AG$3:$AG$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.5000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B8F-4B88-BD03-5D35BA323968}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RED</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AI$3:$AI$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.78</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.84</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.99</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AJ$3:$AJ$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4B8F-4B88-BD03-5D35BA323968}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BLUE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AL$3:$AL$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.63</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.67</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.68</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.83</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AM$3:$AM$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4B8F-4B88-BD03-5D35BA323968}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="712543600"/>
+        <c:axId val="712547440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="712543600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>V(V)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712547440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="712547440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>I(A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712543600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27611142468209438"/>
+          <c:y val="0.9016868078655943"/>
+          <c:w val="0.46784390172948892"/>
+          <c:h val="7.7514000589498519E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6267,6 +7329,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8848,6 +9950,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9584,6 +11202,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>902804</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9C24974-CCEE-C5BB-425D-499D592F3A83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9855,10 +11509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD37"/>
+  <dimension ref="A1:AM37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC52" sqref="AC52"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9873,7 +11527,7 @@
     <col min="29" max="29" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -9919,8 +11573,26 @@
       <c r="AD1" t="s">
         <v>9</v>
       </c>
+      <c r="AF1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9984,8 +11656,26 @@
       <c r="AD2" t="s">
         <v>4</v>
       </c>
+      <c r="AF2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.7</v>
       </c>
@@ -10052,11 +11742,29 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="AD3">
-        <f>AB3*AC3</f>
+        <f t="shared" ref="AD3:AD20" si="0">AB3*AC3</f>
         <v>0.35041000000000005</v>
       </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.65</v>
       </c>
@@ -10064,7 +11772,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C24" si="0">A4*B4</f>
+        <f t="shared" ref="C4:C24" si="1">A4*B4</f>
         <v>0.3503</v>
       </c>
       <c r="E4">
@@ -10084,7 +11792,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K36" si="1">I4*J4</f>
+        <f t="shared" ref="K4:K36" si="2">I4*J4</f>
         <v>0.44428999999999996</v>
       </c>
       <c r="P4">
@@ -10104,7 +11812,7 @@
         <v>0.128</v>
       </c>
       <c r="V4">
-        <f t="shared" ref="V4:V32" si="2">T4*U4</f>
+        <f t="shared" ref="V4:V32" si="3">T4*U4</f>
         <v>0.74112</v>
       </c>
       <c r="X4" s="1">
@@ -10114,7 +11822,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="Z4" s="1">
-        <f>X4*Y4</f>
+        <f t="shared" ref="Z4:Z25" si="4">X4*Y4</f>
         <v>0.17976000000000003</v>
       </c>
       <c r="AB4">
@@ -10124,11 +11832,29 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="AD4">
-        <f>AB4*AC4</f>
+        <f t="shared" si="0"/>
         <v>0.43077000000000004</v>
       </c>
+      <c r="AF4" s="1">
+        <v>1.53</v>
+      </c>
+      <c r="AG4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>1.48</v>
+      </c>
+      <c r="AJ4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="AM4">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.59</v>
       </c>
@@ -10136,7 +11862,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41924999999999996</v>
       </c>
       <c r="E5">
@@ -10146,7 +11872,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G28" si="3">E5*F5</f>
+        <f t="shared" ref="G5:G28" si="5">E5*F5</f>
         <v>0.26695999999999998</v>
       </c>
       <c r="I5">
@@ -10156,7 +11882,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.47725000000000001</v>
       </c>
       <c r="P5">
@@ -10166,7 +11892,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="R5">
-        <f t="shared" ref="R5:R29" si="4">P5*Q5</f>
+        <f t="shared" ref="R5:R29" si="6">P5*Q5</f>
         <v>0.37764999999999999</v>
       </c>
       <c r="T5">
@@ -10176,7 +11902,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="V5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76741000000000004</v>
       </c>
       <c r="X5">
@@ -10186,7 +11912,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="Z5">
-        <f>X5*Y5</f>
+        <f t="shared" si="4"/>
         <v>0.17892</v>
       </c>
       <c r="AB5">
@@ -10196,11 +11922,29 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="AD5">
-        <f>AB5*AC5</f>
+        <f t="shared" si="0"/>
         <v>0.47895000000000004</v>
       </c>
+      <c r="AF5">
+        <v>1.56</v>
+      </c>
+      <c r="AG5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AI5">
+        <v>1.52</v>
+      </c>
+      <c r="AJ5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AL5">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AM5">
+        <v>6.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.53</v>
       </c>
@@ -10208,7 +11952,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.53088000000000002</v>
       </c>
       <c r="E6">
@@ -10218,7 +11962,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.27783000000000002</v>
       </c>
       <c r="I6">
@@ -10228,7 +11972,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.47559000000000007</v>
       </c>
       <c r="P6">
@@ -10238,7 +11982,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="R6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.39507999999999999</v>
       </c>
       <c r="T6">
@@ -10248,7 +11992,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="V6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.83084999999999998</v>
       </c>
       <c r="X6">
@@ -10258,7 +12002,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="Z6">
-        <f>X6*Y6</f>
+        <f t="shared" si="4"/>
         <v>0.16112000000000001</v>
       </c>
       <c r="AB6">
@@ -10268,11 +12012,29 @@
         <v>0.107</v>
       </c>
       <c r="AD6">
-        <f>AB6*AC6</f>
+        <f t="shared" si="0"/>
         <v>0.54569999999999996</v>
       </c>
+      <c r="AF6">
+        <v>1.57</v>
+      </c>
+      <c r="AG6">
+        <v>0.01</v>
+      </c>
+      <c r="AI6">
+        <v>1.54</v>
+      </c>
+      <c r="AJ6">
+        <v>0.01</v>
+      </c>
+      <c r="AL6">
+        <v>2.25</v>
+      </c>
+      <c r="AM6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.51</v>
       </c>
@@ -10280,7 +12042,7 @@
         <v>0.105</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.57855000000000001</v>
       </c>
       <c r="E7">
@@ -10290,7 +12052,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.31752000000000002</v>
       </c>
       <c r="I7">
@@ -10300,7 +12062,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.58241999999999994</v>
       </c>
       <c r="P7">
@@ -10310,7 +12072,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="R7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.41831999999999991</v>
       </c>
       <c r="T7">
@@ -10320,7 +12082,7 @@
         <v>0.16700000000000001</v>
       </c>
       <c r="V7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.95357000000000003</v>
       </c>
       <c r="X7">
@@ -10330,7 +12092,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="Z7">
-        <f>X7*Y7</f>
+        <f t="shared" si="4"/>
         <v>0.14504</v>
       </c>
       <c r="AB7">
@@ -10340,11 +12102,29 @@
         <v>0.114</v>
       </c>
       <c r="AD7">
-        <f>AB7*AC7</f>
+        <f t="shared" si="0"/>
         <v>0.57684000000000002</v>
       </c>
+      <c r="AF7">
+        <v>1.59</v>
+      </c>
+      <c r="AG7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AI7">
+        <v>1.59</v>
+      </c>
+      <c r="AJ7">
+        <v>0.02</v>
+      </c>
+      <c r="AL7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AM7">
+        <v>0.02</v>
+      </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5.43</v>
       </c>
@@ -10352,7 +12132,7 @@
         <v>0.12</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.65159999999999996</v>
       </c>
       <c r="E8">
@@ -10362,7 +12142,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.36854999999999999</v>
       </c>
       <c r="I8">
@@ -10372,7 +12152,7 @@
         <v>0.12</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68280000000000007</v>
       </c>
       <c r="P8">
@@ -10382,7 +12162,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="R8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.47891</v>
       </c>
       <c r="T8">
@@ -10392,7 +12172,7 @@
         <v>0.18</v>
       </c>
       <c r="V8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0206</v>
       </c>
       <c r="X8">
@@ -10402,7 +12182,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="Z8">
-        <f>X8*Y8</f>
+        <f t="shared" si="4"/>
         <v>0.13911999999999999</v>
       </c>
       <c r="AB8">
@@ -10412,11 +12192,29 @@
         <v>0.13</v>
       </c>
       <c r="AD8">
-        <f>AB8*AC8</f>
+        <f t="shared" si="0"/>
         <v>0.65259999999999996</v>
       </c>
+      <c r="AF8">
+        <v>1.6</v>
+      </c>
+      <c r="AG8">
+        <v>0.02</v>
+      </c>
+      <c r="AI8">
+        <v>1.63</v>
+      </c>
+      <c r="AJ8">
+        <v>0.03</v>
+      </c>
+      <c r="AL8">
+        <v>2.35</v>
+      </c>
+      <c r="AM8">
+        <v>0.03</v>
+      </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.33</v>
       </c>
@@ -10424,7 +12222,7 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.73021000000000003</v>
       </c>
       <c r="E9">
@@ -10434,7 +12232,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.42449999999999999</v>
       </c>
       <c r="I9">
@@ -10444,7 +12242,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.78246000000000004</v>
       </c>
       <c r="P9">
@@ -10454,7 +12252,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="R9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.53474999999999995</v>
       </c>
       <c r="T9">
@@ -10464,7 +12262,7 @@
         <v>0.2</v>
       </c>
       <c r="V9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1260000000000001</v>
       </c>
       <c r="X9">
@@ -10474,7 +12272,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="Z9">
-        <f>X9*Y9</f>
+        <f t="shared" si="4"/>
         <v>0.12728</v>
       </c>
       <c r="AB9">
@@ -10484,11 +12282,29 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="AD9">
-        <f>AB9*AC9</f>
+        <f t="shared" si="0"/>
         <v>0.72911999999999999</v>
       </c>
+      <c r="AF9">
+        <v>1.61</v>
+      </c>
+      <c r="AG9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AI9">
+        <v>1.65</v>
+      </c>
+      <c r="AJ9">
+        <v>0.04</v>
+      </c>
+      <c r="AL9">
+        <v>2.39</v>
+      </c>
+      <c r="AM9">
+        <v>0.04</v>
+      </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.21</v>
       </c>
@@ -10496,7 +12312,7 @@
         <v>0.154</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80233999999999994</v>
       </c>
       <c r="E10">
@@ -10506,7 +12322,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.51980000000000004</v>
       </c>
       <c r="I10">
@@ -10516,7 +12332,7 @@
         <v>0.16400000000000001</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92660000000000009</v>
       </c>
       <c r="P10">
@@ -10526,7 +12342,7 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="R10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.59224999999999994</v>
       </c>
       <c r="T10">
@@ -10536,133 +12352,169 @@
         <v>0.20699999999999999</v>
       </c>
       <c r="V10">
+        <f t="shared" si="3"/>
+        <v>1.16127</v>
+      </c>
+      <c r="X10">
+        <v>3.2</v>
+      </c>
+      <c r="Y10">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="4"/>
+        <v>0.11840000000000001</v>
+      </c>
+      <c r="AB10">
+        <v>4.88</v>
+      </c>
+      <c r="AC10">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="0"/>
+        <v>0.81984000000000001</v>
+      </c>
+      <c r="AF10">
+        <v>1.62</v>
+      </c>
+      <c r="AG10">
+        <v>0.03</v>
+      </c>
+      <c r="AI10">
+        <v>1.69</v>
+      </c>
+      <c r="AJ10">
+        <v>0.05</v>
+      </c>
+      <c r="AL10">
+        <v>2.42</v>
+      </c>
+      <c r="AM10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="B11">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.84501999999999999</v>
+      </c>
+      <c r="E11">
+        <v>5.65</v>
+      </c>
+      <c r="F11">
+        <v>0.106</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>0.59889999999999999</v>
+      </c>
+      <c r="I11">
+        <v>5.63</v>
+      </c>
+      <c r="J11">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>1.10911</v>
+      </c>
+      <c r="P11">
+        <v>5.69</v>
+      </c>
+      <c r="Q11">
+        <v>0.113</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="6"/>
+        <v>0.64297000000000004</v>
+      </c>
+      <c r="T11">
+        <v>5.59</v>
+      </c>
+      <c r="U11">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="3"/>
+        <v>1.2689300000000001</v>
+      </c>
+      <c r="X11">
+        <v>2.94</v>
+      </c>
+      <c r="Y11">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="4"/>
+        <v>0.11172</v>
+      </c>
+      <c r="AB11">
+        <v>4.76</v>
+      </c>
+      <c r="AC11">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="0"/>
+        <v>0.96152000000000004</v>
+      </c>
+      <c r="AF11">
+        <v>1.63</v>
+      </c>
+      <c r="AG11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AI11">
+        <v>1.72</v>
+      </c>
+      <c r="AJ11">
+        <v>0.06</v>
+      </c>
+      <c r="AL11">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AM11">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4.92</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="E12">
+        <v>5.67</v>
+      </c>
+      <c r="F12">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>0.65771999999999997</v>
+      </c>
+      <c r="I12">
+        <v>5.61</v>
+      </c>
+      <c r="J12">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="2"/>
         <v>1.16127</v>
       </c>
-      <c r="X10">
-        <v>3.2</v>
-      </c>
-      <c r="Y10">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="Z10">
-        <f>X10*Y10</f>
-        <v>0.11840000000000001</v>
-      </c>
-      <c r="AB10">
-        <v>4.88</v>
-      </c>
-      <c r="AC10">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="AD10">
-        <f>AB10*AC10</f>
-        <v>0.81984000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="B11">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0.84501999999999999</v>
-      </c>
-      <c r="E11">
-        <v>5.65</v>
-      </c>
-      <c r="F11">
-        <v>0.106</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="3"/>
-        <v>0.59889999999999999</v>
-      </c>
-      <c r="I11">
-        <v>5.63</v>
-      </c>
-      <c r="J11">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>1.10911</v>
-      </c>
-      <c r="P11">
-        <v>5.69</v>
-      </c>
-      <c r="Q11">
-        <v>0.113</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="4"/>
-        <v>0.64297000000000004</v>
-      </c>
-      <c r="T11">
-        <v>5.59</v>
-      </c>
-      <c r="U11">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="V11">
-        <f t="shared" si="2"/>
-        <v>1.2689300000000001</v>
-      </c>
-      <c r="X11">
-        <v>2.94</v>
-      </c>
-      <c r="Y11">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="Z11">
-        <f>X11*Y11</f>
-        <v>0.11172</v>
-      </c>
-      <c r="AB11">
-        <v>4.76</v>
-      </c>
-      <c r="AC11">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="AD11">
-        <f>AB11*AC11</f>
-        <v>0.96152000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4.92</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.86099999999999999</v>
-      </c>
-      <c r="E12">
-        <v>5.67</v>
-      </c>
-      <c r="F12">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
-        <v>0.65771999999999997</v>
-      </c>
-      <c r="I12">
-        <v>5.61</v>
-      </c>
-      <c r="J12">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>1.16127</v>
-      </c>
       <c r="P12">
         <v>5.67</v>
       </c>
@@ -10670,7 +12522,7 @@
         <v>0.126</v>
       </c>
       <c r="R12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.71441999999999994</v>
       </c>
       <c r="T12">
@@ -10680,7 +12532,7 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="V12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3312299999999999</v>
       </c>
       <c r="X12">
@@ -10690,7 +12542,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="Z12">
-        <f>X12*Y12</f>
+        <f t="shared" si="4"/>
         <v>0.10563999999999998</v>
       </c>
       <c r="AB12" s="1">
@@ -10700,11 +12552,29 @@
         <v>0.23200000000000001</v>
       </c>
       <c r="AD12" s="1">
-        <f>AB12*AC12</f>
+        <f t="shared" si="0"/>
         <v>1.0811200000000001</v>
       </c>
+      <c r="AF12">
+        <v>1.64</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="AI12">
+        <v>1.75</v>
+      </c>
+      <c r="AJ12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AL12">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="AM12">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4.7</v>
       </c>
@@ -10712,7 +12582,7 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83189999999999997</v>
       </c>
       <c r="E13">
@@ -10722,7 +12592,7 @@
         <v>0.126</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.70938000000000001</v>
       </c>
       <c r="I13">
@@ -10732,7 +12602,7 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3360099999999999</v>
       </c>
       <c r="P13">
@@ -10742,7 +12612,7 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="R13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.76568000000000003</v>
       </c>
       <c r="T13">
@@ -10752,7 +12622,7 @@
         <v>0.25800000000000001</v>
       </c>
       <c r="V13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4319</v>
       </c>
       <c r="X13">
@@ -10762,7 +12632,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="Z13">
-        <f>X13*Y13</f>
+        <f t="shared" si="4"/>
         <v>8.9080000000000006E-2</v>
       </c>
       <c r="AB13">
@@ -10772,11 +12642,29 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="AD13">
-        <f>AB13*AC13</f>
+        <f t="shared" si="0"/>
         <v>1.0648</v>
       </c>
+      <c r="AF13">
+        <v>1.65</v>
+      </c>
+      <c r="AG13">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AI13">
+        <v>1.78</v>
+      </c>
+      <c r="AJ13">
+        <v>0.08</v>
+      </c>
+      <c r="AL13">
+        <v>2.52</v>
+      </c>
+      <c r="AM13">
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4.3600000000000003</v>
       </c>
@@ -10784,7 +12672,7 @@
         <v>0.193</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84148000000000012</v>
       </c>
       <c r="E14">
@@ -10794,7 +12682,7 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.76296000000000008</v>
       </c>
       <c r="I14">
@@ -10804,7 +12692,7 @@
         <v>0.28100000000000003</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5651700000000002</v>
       </c>
       <c r="P14">
@@ -10814,7 +12702,7 @@
         <v>0.14599999999999999</v>
       </c>
       <c r="R14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.81906000000000001</v>
       </c>
       <c r="T14">
@@ -10824,7 +12712,7 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="V14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4599200000000001</v>
       </c>
       <c r="X14">
@@ -10834,7 +12722,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="Z14">
-        <f>X14*Y14</f>
+        <f t="shared" si="4"/>
         <v>8.0500000000000002E-2</v>
       </c>
       <c r="AB14">
@@ -10844,11 +12732,29 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="AD14">
-        <f>AB14*AC14</f>
+        <f t="shared" si="0"/>
         <v>1.0067200000000001</v>
       </c>
+      <c r="AF14">
+        <v>1.66</v>
+      </c>
+      <c r="AG14">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AI14">
+        <v>1.81</v>
+      </c>
+      <c r="AJ14">
+        <v>0.09</v>
+      </c>
+      <c r="AL14">
+        <v>2.54</v>
+      </c>
+      <c r="AM14">
+        <v>0.09</v>
+      </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4.0599999999999996</v>
       </c>
@@ -10856,7 +12762,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.79575999999999991</v>
       </c>
       <c r="E15">
@@ -10866,7 +12772,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.80474999999999997</v>
       </c>
       <c r="I15">
@@ -10876,7 +12782,7 @@
         <v>0.308</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7094</v>
       </c>
       <c r="P15">
@@ -10886,7 +12792,7 @@
         <v>0.154</v>
       </c>
       <c r="R15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.86085999999999996</v>
       </c>
       <c r="T15">
@@ -10896,7 +12802,7 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5703499999999999</v>
       </c>
       <c r="X15">
@@ -10906,7 +12812,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="Z15">
-        <f>X15*Y15</f>
+        <f t="shared" si="4"/>
         <v>6.93E-2</v>
       </c>
       <c r="AB15">
@@ -10916,11 +12822,29 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="AD15">
-        <f>AB15*AC15</f>
+        <f t="shared" si="0"/>
         <v>0.95648</v>
       </c>
+      <c r="AF15">
+        <v>1.68</v>
+      </c>
+      <c r="AG15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AI15">
+        <v>1.84</v>
+      </c>
+      <c r="AJ15">
+        <v>0.1</v>
+      </c>
+      <c r="AL15">
+        <v>2.57</v>
+      </c>
+      <c r="AM15">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3.67</v>
       </c>
@@ -10928,7 +12852,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.71931999999999996</v>
       </c>
       <c r="E16">
@@ -10938,7 +12862,7 @@
         <v>0.156</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.85643999999999998</v>
       </c>
       <c r="I16">
@@ -10948,7 +12872,7 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8954399999999998</v>
       </c>
       <c r="P16">
@@ -10958,7 +12882,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="R16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.92462000000000011</v>
       </c>
       <c r="T16">
@@ -10968,7 +12892,7 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="V16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.62504</v>
       </c>
       <c r="X16">
@@ -10978,7 +12902,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="Z16">
-        <f>X16*Y16</f>
+        <f t="shared" si="4"/>
         <v>6.7979999999999999E-2</v>
       </c>
       <c r="AB16">
@@ -10988,11 +12912,29 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="AD16">
-        <f>AB16*AC16</f>
+        <f t="shared" si="0"/>
         <v>0.91743999999999992</v>
       </c>
+      <c r="AF16">
+        <v>1.69</v>
+      </c>
+      <c r="AG16">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AI16">
+        <v>1.89</v>
+      </c>
+      <c r="AJ16">
+        <v>0.12</v>
+      </c>
+      <c r="AL16">
+        <v>2.59</v>
+      </c>
+      <c r="AM16">
+        <v>0.11</v>
+      </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3.23</v>
       </c>
@@ -11000,7 +12942,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.63307999999999998</v>
       </c>
       <c r="E17">
@@ -11010,7 +12952,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.90254999999999996</v>
       </c>
       <c r="I17">
@@ -11020,7 +12962,7 @@
         <v>0.39400000000000002</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1394199999999999</v>
       </c>
       <c r="P17">
@@ -11030,7 +12972,7 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="R17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.97328000000000003</v>
       </c>
       <c r="T17">
@@ -11040,7 +12982,7 @@
         <v>0.3</v>
       </c>
       <c r="V17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.635</v>
       </c>
       <c r="X17">
@@ -11050,7 +12992,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="Z17">
-        <f>X17*Y17</f>
+        <f t="shared" si="4"/>
         <v>6.2719999999999998E-2</v>
       </c>
       <c r="AB17">
@@ -11060,11 +13002,29 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="AD17">
-        <f>AB17*AC17</f>
+        <f t="shared" si="0"/>
         <v>0.83448</v>
       </c>
+      <c r="AF17">
+        <v>1.7</v>
+      </c>
+      <c r="AG17">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AI17">
+        <v>1.93</v>
+      </c>
+      <c r="AJ17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AL17">
+        <v>2.61</v>
+      </c>
+      <c r="AM17">
+        <v>0.12</v>
+      </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.1</v>
       </c>
@@ -11072,7 +13032,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.60760000000000003</v>
       </c>
       <c r="E18">
@@ -11082,7 +13042,7 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.95216000000000001</v>
       </c>
       <c r="I18">
@@ -11092,7 +13052,7 @@
         <v>0.42199999999999999</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2745799999999998</v>
       </c>
       <c r="P18">
@@ -11102,7 +13062,7 @@
         <v>0.185</v>
       </c>
       <c r="R18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99714999999999998</v>
       </c>
       <c r="T18">
@@ -11112,7 +13072,7 @@
         <v>0.318</v>
       </c>
       <c r="V18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7267399999999999</v>
       </c>
       <c r="X18">
@@ -11122,7 +13082,7 @@
         <v>0.03</v>
       </c>
       <c r="Z18">
-        <f>X18*Y18</f>
+        <f t="shared" si="4"/>
         <v>5.6399999999999992E-2</v>
       </c>
       <c r="AB18">
@@ -11132,11 +13092,29 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="AD18">
-        <f>AB18*AC18</f>
+        <f t="shared" si="0"/>
         <v>0.76302000000000003</v>
       </c>
+      <c r="AF18">
+        <v>1.71</v>
+      </c>
+      <c r="AG18">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AI18">
+        <v>1.98</v>
+      </c>
+      <c r="AJ18">
+        <v>0.16</v>
+      </c>
+      <c r="AL18">
+        <v>2.63</v>
+      </c>
+      <c r="AM18">
+        <v>0.13</v>
+      </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.7</v>
       </c>
@@ -11144,7 +13122,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5292</v>
       </c>
       <c r="E19">
@@ -11154,7 +13132,7 @@
         <v>0.185</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.99714999999999998</v>
       </c>
       <c r="I19">
@@ -11164,7 +13142,7 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4411400000000003</v>
       </c>
       <c r="P19">
@@ -11174,7 +13152,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="R19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0525200000000001</v>
       </c>
       <c r="T19">
@@ -11184,7 +13162,7 @@
         <v>0.34</v>
       </c>
       <c r="V19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8394000000000001</v>
       </c>
       <c r="X19">
@@ -11194,7 +13172,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="Z19">
-        <f>X19*Y19</f>
+        <f t="shared" si="4"/>
         <v>4.5919999999999996E-2</v>
       </c>
       <c r="AB19">
@@ -11204,11 +13182,29 @@
         <v>0.247</v>
       </c>
       <c r="AD19">
-        <f>AB19*AC19</f>
+        <f t="shared" si="0"/>
         <v>0.71135999999999999</v>
       </c>
+      <c r="AF19">
+        <v>1.72</v>
+      </c>
+      <c r="AG19">
+        <v>0.1</v>
+      </c>
+      <c r="AI19">
+        <v>1.99</v>
+      </c>
+      <c r="AJ19">
+        <v>0.18</v>
+      </c>
+      <c r="AL19">
+        <v>2.65</v>
+      </c>
+      <c r="AM19">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.2799999999999998</v>
       </c>
@@ -11216,7 +13212,7 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4446</v>
       </c>
       <c r="E20">
@@ -11226,7 +13222,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0486</v>
       </c>
       <c r="I20">
@@ -11236,7 +13232,7 @@
         <v>0.498</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6145</v>
       </c>
       <c r="P20">
@@ -11246,7 +13242,7 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="R20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0897399999999999</v>
       </c>
       <c r="T20">
@@ -11256,7 +13252,7 @@
         <v>0.36699999999999999</v>
       </c>
       <c r="V20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9781299999999999</v>
       </c>
       <c r="X20">
@@ -11266,7 +13262,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="Z20">
-        <f>X20*Y20</f>
+        <f t="shared" si="4"/>
         <v>4.3680000000000004E-2</v>
       </c>
       <c r="AB20">
@@ -11276,11 +13272,29 @@
         <v>0.249</v>
       </c>
       <c r="AD20">
-        <f>AB20*AC20</f>
+        <f t="shared" si="0"/>
         <v>0.57767999999999997</v>
       </c>
+      <c r="AF20">
+        <v>1.73</v>
+      </c>
+      <c r="AG20">
+        <v>0.11</v>
+      </c>
+      <c r="AI20">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AJ20">
+        <v>0.2</v>
+      </c>
+      <c r="AL20">
+        <v>2.67</v>
+      </c>
+      <c r="AM20">
+        <v>0.15</v>
+      </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.86</v>
       </c>
@@ -11288,7 +13302,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.36642000000000002</v>
       </c>
       <c r="E21">
@@ -11298,7 +13312,7 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1020999999999999</v>
       </c>
       <c r="I21">
@@ -11308,7 +13322,7 @@
         <v>0.53</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7401</v>
       </c>
       <c r="P21">
@@ -11318,7 +13332,7 @@
         <v>0.216</v>
       </c>
       <c r="R21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.12968</v>
       </c>
       <c r="T21">
@@ -11328,7 +13342,7 @@
         <v>0.39</v>
       </c>
       <c r="V21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.0865</v>
       </c>
       <c r="X21">
@@ -11338,11 +13352,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Z21">
-        <f>X21*Y21</f>
+        <f t="shared" si="4"/>
         <v>3.0499999999999999E-2</v>
       </c>
+      <c r="AF21">
+        <v>1.74</v>
+      </c>
+      <c r="AG21">
+        <v>0.12</v>
+      </c>
+      <c r="AI21">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="AJ21">
+        <v>0.22</v>
+      </c>
+      <c r="AL21">
+        <v>2.68</v>
+      </c>
+      <c r="AM21">
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.3</v>
       </c>
@@ -11350,7 +13382,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25609999999999999</v>
       </c>
       <c r="E22">
@@ -11360,7 +13392,7 @@
         <v>0.216</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.14696</v>
       </c>
       <c r="I22">
@@ -11370,7 +13402,7 @@
         <v>0.59099999999999997</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9077199999999999</v>
       </c>
       <c r="P22">
@@ -11380,7 +13412,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="R22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.16842</v>
       </c>
       <c r="T22">
@@ -11390,7 +13422,7 @@
         <v>0.41</v>
       </c>
       <c r="V22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.1852999999999998</v>
       </c>
       <c r="X22">
@@ -11400,11 +13432,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Z22">
-        <f>X22*Y22</f>
+        <f t="shared" si="4"/>
         <v>2.6000000000000002E-2</v>
       </c>
+      <c r="AF22">
+        <v>1.75</v>
+      </c>
+      <c r="AG22">
+        <v>0.13</v>
+      </c>
+      <c r="AI22">
+        <v>2.14</v>
+      </c>
+      <c r="AJ22">
+        <v>0.24</v>
+      </c>
+      <c r="AL22">
+        <v>2.7</v>
+      </c>
+      <c r="AM22">
+        <v>0.17</v>
+      </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.92</v>
       </c>
@@ -11412,7 +13462,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.18124000000000001</v>
       </c>
       <c r="E23">
@@ -11422,7 +13472,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.18198</v>
       </c>
       <c r="I23">
@@ -11432,7 +13482,7 @@
         <v>0.61099999999999999</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.94502</v>
       </c>
       <c r="P23">
@@ -11442,7 +13492,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="R23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.21068</v>
       </c>
       <c r="T23">
@@ -11452,7 +13502,7 @@
         <v>0.433</v>
       </c>
       <c r="V23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.2992299999999997</v>
       </c>
       <c r="X23">
@@ -11462,11 +13512,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Z23">
-        <f>X23*Y23</f>
+        <f t="shared" si="4"/>
         <v>2.1000000000000001E-2</v>
       </c>
+      <c r="AF23">
+        <v>1.77</v>
+      </c>
+      <c r="AG23">
+        <v>0.15</v>
+      </c>
+      <c r="AI23">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="AJ23">
+        <v>0.26</v>
+      </c>
+      <c r="AL23">
+        <v>2.71</v>
+      </c>
+      <c r="AM23">
+        <v>0.18</v>
+      </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.8</v>
       </c>
@@ -11474,7 +13542,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15760000000000002</v>
       </c>
       <c r="E24" s="1">
@@ -11484,7 +13552,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2154</v>
       </c>
       <c r="I24" s="1">
@@ -11494,7 +13562,7 @@
         <v>0.64400000000000002</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9495200000000001</v>
       </c>
       <c r="P24">
@@ -11504,7 +13572,7 @@
         <v>0.246</v>
       </c>
       <c r="R24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2545999999999999</v>
       </c>
       <c r="T24">
@@ -11514,7 +13582,7 @@
         <v>0.46400000000000002</v>
       </c>
       <c r="V24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4452799999999999</v>
       </c>
       <c r="X24">
@@ -11524,11 +13592,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Z24">
-        <f>X24*Y24</f>
+        <f t="shared" si="4"/>
         <v>1.7499999999999998E-2</v>
       </c>
+      <c r="AF24">
+        <v>1.79</v>
+      </c>
+      <c r="AG24">
+        <v>0.17</v>
+      </c>
+      <c r="AI24">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AJ24">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AL24">
+        <v>2.73</v>
+      </c>
+      <c r="AM24">
+        <v>0.19</v>
+      </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>4.96</v>
       </c>
@@ -11536,7 +13622,7 @@
         <v>0.24</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1903999999999999</v>
       </c>
       <c r="I25">
@@ -11546,7 +13632,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9115000000000002</v>
       </c>
       <c r="P25">
@@ -11556,7 +13642,7 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="R25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3004800000000001</v>
       </c>
       <c r="T25" s="2">
@@ -11566,7 +13652,7 @@
         <v>0.48499999999999999</v>
       </c>
       <c r="V25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.5462500000000001</v>
       </c>
       <c r="X25">
@@ -11576,11 +13662,23 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Z25">
-        <f>X25*Y25</f>
+        <f t="shared" si="4"/>
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="AF25">
+        <v>1.82</v>
+      </c>
+      <c r="AG25">
+        <v>0.2</v>
+      </c>
+      <c r="AL25">
+        <v>2.74</v>
+      </c>
+      <c r="AM25">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>4.6399999999999997</v>
       </c>
@@ -11588,7 +13686,7 @@
         <v>0.245</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1367999999999998</v>
       </c>
       <c r="I26">
@@ -11598,7 +13696,7 @@
         <v>0.65</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.8340000000000005</v>
       </c>
       <c r="P26" s="1">
@@ -11608,7 +13706,7 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="R26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3038000000000001</v>
       </c>
       <c r="T26">
@@ -11618,11 +13716,23 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="V26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7039900000000001</v>
       </c>
+      <c r="AF26">
+        <v>1.84</v>
+      </c>
+      <c r="AG26">
+        <v>0.22</v>
+      </c>
+      <c r="AL26">
+        <v>2.77</v>
+      </c>
+      <c r="AM26">
+        <v>0.22</v>
+      </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>3.84</v>
       </c>
@@ -11630,7 +13740,7 @@
         <v>0.246</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.94463999999999992</v>
       </c>
       <c r="I27">
@@ -11640,7 +13750,7 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.8158599999999998</v>
       </c>
       <c r="P27">
@@ -11650,7 +13760,7 @@
         <v>0.27700000000000002</v>
       </c>
       <c r="R27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3129800000000003</v>
       </c>
       <c r="T27">
@@ -11660,11 +13770,23 @@
         <v>0.54300000000000004</v>
       </c>
       <c r="V27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.8181700000000003</v>
       </c>
+      <c r="AF27">
+        <v>1.86</v>
+      </c>
+      <c r="AG27">
+        <v>0.24</v>
+      </c>
+      <c r="AL27">
+        <v>2.8</v>
+      </c>
+      <c r="AM27">
+        <v>0.24</v>
+      </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>2.66</v>
       </c>
@@ -11672,7 +13794,7 @@
         <v>0.25</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.66500000000000004</v>
       </c>
       <c r="I28">
@@ -11682,7 +13804,7 @@
         <v>0.66700000000000004</v>
       </c>
       <c r="K28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7347000000000001</v>
       </c>
       <c r="P28">
@@ -11692,7 +13814,7 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="R28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3213199999999998</v>
       </c>
       <c r="T28">
@@ -11702,11 +13824,23 @@
         <v>0.58299999999999996</v>
       </c>
       <c r="V28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9907899999999996</v>
       </c>
+      <c r="AF28">
+        <v>1.88</v>
+      </c>
+      <c r="AG28">
+        <v>0.26</v>
+      </c>
+      <c r="AL28">
+        <v>2.83</v>
+      </c>
+      <c r="AM28">
+        <v>0.26</v>
+      </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I29">
         <v>4</v>
       </c>
@@ -11714,7 +13848,7 @@
         <v>0.67100000000000004</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6840000000000002</v>
       </c>
       <c r="P29">
@@ -11724,7 +13858,7 @@
         <v>0.29199999999999998</v>
       </c>
       <c r="R29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.80008000000000001</v>
       </c>
       <c r="T29">
@@ -11734,11 +13868,23 @@
         <v>0.60699999999999998</v>
       </c>
       <c r="V29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0956999999999999</v>
       </c>
+      <c r="AF29">
+        <v>1.9</v>
+      </c>
+      <c r="AG29">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AL29">
+        <v>2.85</v>
+      </c>
+      <c r="AM29">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I30">
         <v>3.9</v>
       </c>
@@ -11746,7 +13892,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6793</v>
       </c>
       <c r="T30">
@@ -11756,11 +13902,11 @@
         <v>0.63600000000000001</v>
       </c>
       <c r="V30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.2054400000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I31">
         <v>3.6</v>
       </c>
@@ -11768,7 +13914,7 @@
         <v>0.68200000000000005</v>
       </c>
       <c r="K31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4552</v>
       </c>
       <c r="T31" s="1">
@@ -11778,11 +13924,11 @@
         <v>0.65900000000000003</v>
       </c>
       <c r="V31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.26864</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I32">
         <v>3.54</v>
       </c>
@@ -11790,7 +13936,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="K32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4319800000000003</v>
       </c>
       <c r="T32">
@@ -11800,7 +13946,7 @@
         <v>0.65900000000000003</v>
       </c>
       <c r="V32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1829700000000001</v>
       </c>
     </row>
@@ -11812,7 +13958,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.36328</v>
       </c>
       <c r="T33">
@@ -11834,7 +13980,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.28084</v>
       </c>
       <c r="T34">
@@ -11856,7 +14002,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="K35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0884800000000001</v>
       </c>
       <c r="T35">
@@ -11878,7 +14024,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="K36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7312400000000001</v>
       </c>
       <c r="T36">

</xml_diff>

<commit_message>
Update LED driver code
</commit_message>
<xml_diff>
--- a/Power/Measurements.xlsx
+++ b/Power/Measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\YEAR 2\PROJECT\power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EFC976-002B-4419-A6CF-441593E14464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867702A1-60AF-4E96-B7F2-B8A1D3AB7531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="5580" windowWidth="23085" windowHeight="10485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
   <si>
     <t>V</t>
   </si>
@@ -91,6 +91,24 @@
   <si>
     <t>BLUE</t>
   </si>
+  <si>
+    <t>DURATIION TEST</t>
+  </si>
+  <si>
+    <t>29/5/2023</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
 </sst>
 </file>
 
@@ -138,10 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -198,7 +217,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t> Curve of 3-Pannel</a:t>
+              <a:t> Curve of 3-Panel</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
@@ -1265,7 +1284,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>I-V Curve of 3-Pannel</a:t>
+              <a:t>I-V Curve of 3-Panel</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2363,7 +2382,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>I-V Curve of 1-Pannel Sunny</a:t>
+              <a:t>I-V Curve of 1-Panel Sunny</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2939,7 +2958,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t> Curve of 1-Pannel Sunny</a:t>
+              <a:t> Curve of 1-Panel Sunny</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" altLang="zh-CN"/>
           </a:p>
@@ -2949,8 +2968,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20843744531933509"/>
-          <c:y val="2.3148148148148147E-2"/>
+          <c:x val="0.21404003005055042"/>
+          <c:y val="2.3148143082093071E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3516,7 +3535,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t> Curve of 3-Panne</a:t>
+              <a:t> Curve of 3-Panel</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
@@ -4289,58 +4308,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>5.23</c:v>
+                  <c:v>5.53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.19</c:v>
+                  <c:v>5.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.15</c:v>
+                  <c:v>5.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0999999999999996</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>5.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>5.0599999999999996</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>4.96</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.88</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.76</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.66</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.16</c:v>
+                  <c:v>4.46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.92</c:v>
+                  <c:v>4.22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.76</c:v>
+                  <c:v>4.0599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.42</c:v>
+                  <c:v>3.72</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.14</c:v>
+                  <c:v>3.44</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.88</c:v>
+                  <c:v>3.18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3199999999999998</c:v>
+                  <c:v>2.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4780,7 +4799,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>I-V Curve of 3-Pannel</a:t>
+              <a:t>P-V Curve of 3-Panel</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5570,58 +5589,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>5.23</c:v>
+                  <c:v>5.53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.19</c:v>
+                  <c:v>5.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.15</c:v>
+                  <c:v>5.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0999999999999996</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>5.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>5.0599999999999996</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>4.96</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.88</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.76</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.66</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.16</c:v>
+                  <c:v>4.46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.92</c:v>
+                  <c:v>4.22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.76</c:v>
+                  <c:v>4.0599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.42</c:v>
+                  <c:v>3.72</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.14</c:v>
+                  <c:v>3.44</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.88</c:v>
+                  <c:v>3.18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3199999999999998</c:v>
+                  <c:v>2.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5633,58 +5652,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.35041000000000005</c:v>
+                  <c:v>0.37051000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43077000000000004</c:v>
+                  <c:v>0.45567000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47895000000000004</c:v>
+                  <c:v>0.50685000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54569999999999996</c:v>
+                  <c:v>0.57779999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57684000000000002</c:v>
+                  <c:v>0.61104000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.65259999999999996</c:v>
+                  <c:v>0.6916000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.72911999999999999</c:v>
+                  <c:v>0.77321999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81984000000000001</c:v>
+                  <c:v>0.87024000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.96152000000000004</c:v>
+                  <c:v>1.0221199999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0811200000000001</c:v>
+                  <c:v>1.15072</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0648</c:v>
+                  <c:v>1.1374</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0067200000000001</c:v>
+                  <c:v>1.0793200000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.95648</c:v>
+                  <c:v>1.0296799999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.91743999999999992</c:v>
+                  <c:v>0.99063999999999985</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.83448</c:v>
+                  <c:v>0.90768000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.76302000000000003</c:v>
+                  <c:v>0.83592</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.71135999999999999</c:v>
+                  <c:v>0.78546000000000005</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.57767999999999997</c:v>
+                  <c:v>0.65238000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6168,82 +6187,82 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.53</c:v>
+                  <c:v>1.83</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.56</c:v>
+                  <c:v>1.86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.57</c:v>
+                  <c:v>1.87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.59</c:v>
+                  <c:v>1.89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.61</c:v>
+                  <c:v>1.91</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.62</c:v>
+                  <c:v>1.91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.63</c:v>
+                  <c:v>1.93</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.64</c:v>
+                  <c:v>1.94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.65</c:v>
+                  <c:v>1.95</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.66</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.68</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.69</c:v>
+                  <c:v>1.99</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.71</c:v>
+                  <c:v>2.0099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.72</c:v>
+                  <c:v>2.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.73</c:v>
+                  <c:v>2.0299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.74</c:v>
+                  <c:v>2.04</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.75</c:v>
+                  <c:v>2.0499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.77</c:v>
+                  <c:v>2.0699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.79</c:v>
+                  <c:v>2.09</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.82</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.84</c:v>
+                  <c:v>2.14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.86</c:v>
+                  <c:v>2.16</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.88</c:v>
+                  <c:v>2.1800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.9</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6385,67 +6404,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.48</c:v>
+                  <c:v>1.78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.52</c:v>
+                  <c:v>1.82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.54</c:v>
+                  <c:v>1.84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.59</c:v>
+                  <c:v>1.89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.63</c:v>
+                  <c:v>1.93</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.65</c:v>
+                  <c:v>1.95</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.69</c:v>
+                  <c:v>1.99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.72</c:v>
+                  <c:v>2.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.75</c:v>
+                  <c:v>2.0499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.78</c:v>
+                  <c:v>2.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.81</c:v>
+                  <c:v>2.11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.84</c:v>
+                  <c:v>2.14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.89</c:v>
+                  <c:v>2.19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.93</c:v>
+                  <c:v>2.23</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.98</c:v>
+                  <c:v>2.2799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.99</c:v>
+                  <c:v>2.29</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0299999999999998</c:v>
+                  <c:v>2.33</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0699999999999998</c:v>
+                  <c:v>2.37</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.14</c:v>
+                  <c:v>2.44</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1800000000000002</c:v>
+                  <c:v>2.48</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.2200000000000002</c:v>
+                  <c:v>2.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6572,82 +6591,82 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.19</c:v>
+                  <c:v>2.4900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2200000000000002</c:v>
+                  <c:v>2.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.25</c:v>
+                  <c:v>2.5499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.35</c:v>
+                  <c:v>2.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.39</c:v>
+                  <c:v>2.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.42</c:v>
+                  <c:v>2.72</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4900000000000002</c:v>
+                  <c:v>2.79</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.52</c:v>
+                  <c:v>2.82</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.54</c:v>
+                  <c:v>2.84</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.57</c:v>
+                  <c:v>2.87</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.59</c:v>
+                  <c:v>2.89</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.61</c:v>
+                  <c:v>2.91</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.63</c:v>
+                  <c:v>2.93</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.65</c:v>
+                  <c:v>2.95</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.67</c:v>
+                  <c:v>2.97</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.68</c:v>
+                  <c:v>2.98</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.71</c:v>
+                  <c:v>3.01</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.73</c:v>
+                  <c:v>3.03</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.74</c:v>
+                  <c:v>3.04</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.77</c:v>
+                  <c:v>3.07</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.8</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.83</c:v>
+                  <c:v>3.13</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.85</c:v>
+                  <c:v>3.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11509,10 +11528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM37"/>
+  <dimension ref="A1:AQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI4" sqref="AI4"/>
+    <sheetView tabSelected="1" topLeftCell="J13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11525,9 +11544,11 @@
     <col min="16" max="16" width="18.140625" customWidth="1"/>
     <col min="20" max="20" width="16.85546875" customWidth="1"/>
     <col min="29" max="29" width="16.85546875" customWidth="1"/>
+    <col min="41" max="41" width="18.7109375" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -11591,8 +11612,17 @@
       <c r="AM1" t="s">
         <v>17</v>
       </c>
+      <c r="AO1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -11674,8 +11704,17 @@
       <c r="AM2" t="s">
         <v>1</v>
       </c>
+      <c r="AO2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.7</v>
       </c>
@@ -11736,14 +11775,14 @@
         <v>0</v>
       </c>
       <c r="AB3">
-        <v>5.23</v>
+        <v>5.53</v>
       </c>
       <c r="AC3">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="AD3">
         <f t="shared" ref="AD3:AD20" si="0">AB3*AC3</f>
-        <v>0.35041000000000005</v>
+        <v>0.37051000000000006</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -11763,8 +11802,17 @@
       <c r="AM3">
         <v>0</v>
       </c>
+      <c r="AO3" s="3">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="AP3">
+        <v>16</v>
+      </c>
+      <c r="AQ3">
+        <v>5.59</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.65</v>
       </c>
@@ -11826,35 +11874,44 @@
         <v>0.17976000000000003</v>
       </c>
       <c r="AB4">
-        <v>5.19</v>
+        <v>5.49</v>
       </c>
       <c r="AC4">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="AD4">
         <f t="shared" si="0"/>
-        <v>0.43077000000000004</v>
+        <v>0.45567000000000002</v>
       </c>
       <c r="AF4" s="1">
-        <v>1.53</v>
+        <v>1.83</v>
       </c>
       <c r="AG4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AI4" s="1">
-        <v>1.48</v>
+        <v>1.78</v>
       </c>
       <c r="AJ4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AL4" s="1">
-        <v>2.19</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="AM4">
         <v>3.0000000000000001E-3</v>
       </c>
+      <c r="AO4" s="3">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="AP4">
+        <v>15.96</v>
+      </c>
+      <c r="AQ4">
+        <v>5.55</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.59</v>
       </c>
@@ -11916,35 +11973,44 @@
         <v>0.17892</v>
       </c>
       <c r="AB5">
-        <v>5.15</v>
+        <v>5.45</v>
       </c>
       <c r="AC5">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="AD5">
         <f t="shared" si="0"/>
-        <v>0.47895000000000004</v>
+        <v>0.50685000000000002</v>
       </c>
       <c r="AF5">
-        <v>1.56</v>
+        <v>1.86</v>
       </c>
       <c r="AG5">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="AI5">
-        <v>1.52</v>
+        <v>1.82</v>
       </c>
       <c r="AJ5">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="AL5">
-        <v>2.2200000000000002</v>
+        <v>2.52</v>
       </c>
       <c r="AM5">
         <v>6.0000000000000001E-3</v>
       </c>
+      <c r="AO5" s="3">
+        <v>0.65902777777777777</v>
+      </c>
+      <c r="AP5">
+        <v>16.04</v>
+      </c>
+      <c r="AQ5">
+        <v>5.61</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.53</v>
       </c>
@@ -12006,35 +12072,44 @@
         <v>0.16112000000000001</v>
       </c>
       <c r="AB6">
-        <v>5.0999999999999996</v>
+        <v>5.4</v>
       </c>
       <c r="AC6">
         <v>0.107</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>0.54569999999999996</v>
+        <v>0.57779999999999998</v>
       </c>
       <c r="AF6">
-        <v>1.57</v>
+        <v>1.87</v>
       </c>
       <c r="AG6">
         <v>0.01</v>
       </c>
       <c r="AI6">
-        <v>1.54</v>
+        <v>1.84</v>
       </c>
       <c r="AJ6">
         <v>0.01</v>
       </c>
       <c r="AL6">
-        <v>2.25</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="AM6">
         <v>0.01</v>
       </c>
+      <c r="AO6" s="3">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="AP6">
+        <v>16</v>
+      </c>
+      <c r="AQ6">
+        <v>5.63</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.51</v>
       </c>
@@ -12096,35 +12171,44 @@
         <v>0.14504</v>
       </c>
       <c r="AB7">
-        <v>5.0599999999999996</v>
+        <v>5.36</v>
       </c>
       <c r="AC7">
         <v>0.114</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>0.57684000000000002</v>
+        <v>0.61104000000000003</v>
       </c>
       <c r="AF7">
-        <v>1.59</v>
+        <v>1.89</v>
       </c>
       <c r="AG7">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="AI7">
-        <v>1.59</v>
+        <v>1.89</v>
       </c>
       <c r="AJ7">
         <v>0.02</v>
       </c>
       <c r="AL7">
-        <v>2.2999999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="AM7">
         <v>0.02</v>
       </c>
+      <c r="AO7" s="3">
+        <v>0.74236111111111114</v>
+      </c>
+      <c r="AP7">
+        <v>16</v>
+      </c>
+      <c r="AQ7">
+        <v>5.63</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5.43</v>
       </c>
@@ -12186,35 +12270,44 @@
         <v>0.13911999999999999</v>
       </c>
       <c r="AB8">
-        <v>5.0199999999999996</v>
+        <v>5.32</v>
       </c>
       <c r="AC8">
         <v>0.13</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>0.65259999999999996</v>
+        <v>0.6916000000000001</v>
       </c>
       <c r="AF8">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="AG8">
         <v>0.02</v>
       </c>
       <c r="AI8">
-        <v>1.63</v>
+        <v>1.93</v>
       </c>
       <c r="AJ8">
         <v>0.03</v>
       </c>
       <c r="AL8">
-        <v>2.35</v>
+        <v>2.65</v>
       </c>
       <c r="AM8">
         <v>0.03</v>
       </c>
+      <c r="AO8" s="3">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="AP8">
+        <v>16.02</v>
+      </c>
+      <c r="AQ8">
+        <v>5.65</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.33</v>
       </c>
@@ -12276,35 +12369,44 @@
         <v>0.12728</v>
       </c>
       <c r="AB9">
-        <v>4.96</v>
+        <v>5.26</v>
       </c>
       <c r="AC9">
         <v>0.14699999999999999</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>0.72911999999999999</v>
+        <v>0.77321999999999991</v>
       </c>
       <c r="AF9">
-        <v>1.61</v>
+        <v>1.91</v>
       </c>
       <c r="AG9">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="AI9">
-        <v>1.65</v>
+        <v>1.95</v>
       </c>
       <c r="AJ9">
         <v>0.04</v>
       </c>
       <c r="AL9">
-        <v>2.39</v>
+        <v>2.69</v>
       </c>
       <c r="AM9">
         <v>0.04</v>
       </c>
+      <c r="AO9" s="3">
+        <v>0.8256944444444444</v>
+      </c>
+      <c r="AP9">
+        <v>16</v>
+      </c>
+      <c r="AQ9">
+        <v>5.51</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.21</v>
       </c>
@@ -12366,35 +12468,44 @@
         <v>0.11840000000000001</v>
       </c>
       <c r="AB10">
-        <v>4.88</v>
+        <v>5.18</v>
       </c>
       <c r="AC10">
         <v>0.16800000000000001</v>
       </c>
       <c r="AD10">
         <f t="shared" si="0"/>
-        <v>0.81984000000000001</v>
+        <v>0.87024000000000001</v>
       </c>
       <c r="AF10">
-        <v>1.62</v>
+        <v>1.91</v>
       </c>
       <c r="AG10">
         <v>0.03</v>
       </c>
       <c r="AI10">
-        <v>1.69</v>
+        <v>1.99</v>
       </c>
       <c r="AJ10">
         <v>0.05</v>
       </c>
       <c r="AL10">
-        <v>2.42</v>
+        <v>2.72</v>
       </c>
       <c r="AM10">
         <v>0.05</v>
       </c>
+      <c r="AO10" s="3">
+        <v>0.86736111111111114</v>
+      </c>
+      <c r="AP10">
+        <v>11.35</v>
+      </c>
+      <c r="AQ10">
+        <v>4.54</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5.0599999999999996</v>
       </c>
@@ -12456,35 +12567,44 @@
         <v>0.11172</v>
       </c>
       <c r="AB11">
-        <v>4.76</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="AC11">
         <v>0.20200000000000001</v>
       </c>
       <c r="AD11">
         <f t="shared" si="0"/>
-        <v>0.96152000000000004</v>
+        <v>1.0221199999999999</v>
       </c>
       <c r="AF11">
-        <v>1.63</v>
+        <v>1.93</v>
       </c>
       <c r="AG11">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="AI11">
-        <v>1.72</v>
+        <v>2.02</v>
       </c>
       <c r="AJ11">
         <v>0.06</v>
       </c>
       <c r="AL11">
-        <v>2.4500000000000002</v>
+        <v>2.75</v>
       </c>
       <c r="AM11">
         <v>0.06</v>
       </c>
+      <c r="AO11" s="3">
+        <v>0.90902777777777777</v>
+      </c>
+      <c r="AP11">
+        <v>4.72</v>
+      </c>
+      <c r="AQ11">
+        <v>0.06</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4.92</v>
       </c>
@@ -12546,35 +12666,44 @@
         <v>0.10563999999999998</v>
       </c>
       <c r="AB12" s="1">
-        <v>4.66</v>
+        <v>4.96</v>
       </c>
       <c r="AC12" s="1">
         <v>0.23200000000000001</v>
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="0"/>
-        <v>1.0811200000000001</v>
+        <v>1.15072</v>
       </c>
       <c r="AF12">
-        <v>1.64</v>
+        <v>1.94</v>
       </c>
       <c r="AG12" s="2">
         <v>0.04</v>
       </c>
       <c r="AI12">
-        <v>1.75</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="AJ12">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AL12">
-        <v>2.4900000000000002</v>
+        <v>2.79</v>
       </c>
       <c r="AM12">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="AO12" s="3">
+        <v>0.9506944444444444</v>
+      </c>
+      <c r="AP12">
+        <v>1.32</v>
+      </c>
+      <c r="AQ12">
+        <v>0.04</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4.7</v>
       </c>
@@ -12636,35 +12765,35 @@
         <v>8.9080000000000006E-2</v>
       </c>
       <c r="AB13">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="AC13">
         <v>0.24199999999999999</v>
       </c>
       <c r="AD13">
         <f t="shared" si="0"/>
-        <v>1.0648</v>
+        <v>1.1374</v>
       </c>
       <c r="AF13">
-        <v>1.65</v>
+        <v>1.95</v>
       </c>
       <c r="AG13">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="AI13">
-        <v>1.78</v>
+        <v>2.08</v>
       </c>
       <c r="AJ13">
         <v>0.08</v>
       </c>
       <c r="AL13">
-        <v>2.52</v>
+        <v>2.82</v>
       </c>
       <c r="AM13">
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4.3600000000000003</v>
       </c>
@@ -12726,35 +12855,35 @@
         <v>8.0500000000000002E-2</v>
       </c>
       <c r="AB14">
-        <v>4.16</v>
+        <v>4.46</v>
       </c>
       <c r="AC14">
         <v>0.24199999999999999</v>
       </c>
       <c r="AD14">
         <f t="shared" si="0"/>
-        <v>1.0067200000000001</v>
+        <v>1.0793200000000001</v>
       </c>
       <c r="AF14">
-        <v>1.66</v>
+        <v>1.96</v>
       </c>
       <c r="AG14">
         <v>5.5E-2</v>
       </c>
       <c r="AI14">
-        <v>1.81</v>
+        <v>2.11</v>
       </c>
       <c r="AJ14">
         <v>0.09</v>
       </c>
       <c r="AL14">
-        <v>2.54</v>
+        <v>2.84</v>
       </c>
       <c r="AM14">
         <v>0.09</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4.0599999999999996</v>
       </c>
@@ -12816,35 +12945,35 @@
         <v>6.93E-2</v>
       </c>
       <c r="AB15">
-        <v>3.92</v>
+        <v>4.22</v>
       </c>
       <c r="AC15">
         <v>0.24399999999999999</v>
       </c>
       <c r="AD15">
         <f t="shared" si="0"/>
-        <v>0.95648</v>
+        <v>1.0296799999999999</v>
       </c>
       <c r="AF15">
-        <v>1.68</v>
+        <v>1.98</v>
       </c>
       <c r="AG15">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AI15">
-        <v>1.84</v>
+        <v>2.14</v>
       </c>
       <c r="AJ15">
         <v>0.1</v>
       </c>
       <c r="AL15">
-        <v>2.57</v>
+        <v>2.87</v>
       </c>
       <c r="AM15">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3.67</v>
       </c>
@@ -12906,29 +13035,29 @@
         <v>6.7979999999999999E-2</v>
       </c>
       <c r="AB16">
-        <v>3.76</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="AC16">
         <v>0.24399999999999999</v>
       </c>
       <c r="AD16">
         <f t="shared" si="0"/>
-        <v>0.91743999999999992</v>
+        <v>0.99063999999999985</v>
       </c>
       <c r="AF16">
-        <v>1.69</v>
+        <v>1.99</v>
       </c>
       <c r="AG16">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AI16">
-        <v>1.89</v>
+        <v>2.19</v>
       </c>
       <c r="AJ16">
         <v>0.12</v>
       </c>
       <c r="AL16">
-        <v>2.59</v>
+        <v>2.89</v>
       </c>
       <c r="AM16">
         <v>0.11</v>
@@ -12996,29 +13125,29 @@
         <v>6.2719999999999998E-2</v>
       </c>
       <c r="AB17">
-        <v>3.42</v>
+        <v>3.72</v>
       </c>
       <c r="AC17">
         <v>0.24399999999999999</v>
       </c>
       <c r="AD17">
         <f t="shared" si="0"/>
-        <v>0.83448</v>
+        <v>0.90768000000000004</v>
       </c>
       <c r="AF17">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="AG17">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="AI17">
-        <v>1.93</v>
+        <v>2.23</v>
       </c>
       <c r="AJ17">
         <v>0.14000000000000001</v>
       </c>
       <c r="AL17">
-        <v>2.61</v>
+        <v>2.91</v>
       </c>
       <c r="AM17">
         <v>0.12</v>
@@ -13086,29 +13215,29 @@
         <v>5.6399999999999992E-2</v>
       </c>
       <c r="AB18">
-        <v>3.14</v>
+        <v>3.44</v>
       </c>
       <c r="AC18">
         <v>0.24299999999999999</v>
       </c>
       <c r="AD18">
         <f t="shared" si="0"/>
-        <v>0.76302000000000003</v>
+        <v>0.83592</v>
       </c>
       <c r="AF18">
-        <v>1.71</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="AG18">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="AI18">
-        <v>1.98</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="AJ18">
         <v>0.16</v>
       </c>
       <c r="AL18">
-        <v>2.63</v>
+        <v>2.93</v>
       </c>
       <c r="AM18">
         <v>0.13</v>
@@ -13176,29 +13305,29 @@
         <v>4.5919999999999996E-2</v>
       </c>
       <c r="AB19">
-        <v>2.88</v>
+        <v>3.18</v>
       </c>
       <c r="AC19">
         <v>0.247</v>
       </c>
       <c r="AD19">
         <f t="shared" si="0"/>
-        <v>0.71135999999999999</v>
+        <v>0.78546000000000005</v>
       </c>
       <c r="AF19">
-        <v>1.72</v>
+        <v>2.02</v>
       </c>
       <c r="AG19">
         <v>0.1</v>
       </c>
       <c r="AI19">
-        <v>1.99</v>
+        <v>2.29</v>
       </c>
       <c r="AJ19">
         <v>0.18</v>
       </c>
       <c r="AL19">
-        <v>2.65</v>
+        <v>2.95</v>
       </c>
       <c r="AM19">
         <v>0.14000000000000001</v>
@@ -13266,29 +13395,29 @@
         <v>4.3680000000000004E-2</v>
       </c>
       <c r="AB20">
-        <v>2.3199999999999998</v>
+        <v>2.62</v>
       </c>
       <c r="AC20">
         <v>0.249</v>
       </c>
       <c r="AD20">
         <f t="shared" si="0"/>
-        <v>0.57767999999999997</v>
+        <v>0.65238000000000007</v>
       </c>
       <c r="AF20">
-        <v>1.73</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="AG20">
         <v>0.11</v>
       </c>
       <c r="AI20">
-        <v>2.0299999999999998</v>
+        <v>2.33</v>
       </c>
       <c r="AJ20">
         <v>0.2</v>
       </c>
       <c r="AL20">
-        <v>2.67</v>
+        <v>2.97</v>
       </c>
       <c r="AM20">
         <v>0.15</v>
@@ -13356,19 +13485,19 @@
         <v>3.0499999999999999E-2</v>
       </c>
       <c r="AF21">
-        <v>1.74</v>
+        <v>2.04</v>
       </c>
       <c r="AG21">
         <v>0.12</v>
       </c>
       <c r="AI21">
-        <v>2.0699999999999998</v>
+        <v>2.37</v>
       </c>
       <c r="AJ21">
         <v>0.22</v>
       </c>
       <c r="AL21">
-        <v>2.68</v>
+        <v>2.98</v>
       </c>
       <c r="AM21">
         <v>0.16</v>
@@ -13436,19 +13565,19 @@
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="AF22">
-        <v>1.75</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="AG22">
         <v>0.13</v>
       </c>
       <c r="AI22">
-        <v>2.14</v>
+        <v>2.44</v>
       </c>
       <c r="AJ22">
         <v>0.24</v>
       </c>
       <c r="AL22">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="AM22">
         <v>0.17</v>
@@ -13516,19 +13645,19 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="AF23">
-        <v>1.77</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="AG23">
         <v>0.15</v>
       </c>
       <c r="AI23">
-        <v>2.1800000000000002</v>
+        <v>2.48</v>
       </c>
       <c r="AJ23">
         <v>0.26</v>
       </c>
       <c r="AL23">
-        <v>2.71</v>
+        <v>3.01</v>
       </c>
       <c r="AM23">
         <v>0.18</v>
@@ -13596,19 +13725,19 @@
         <v>1.7499999999999998E-2</v>
       </c>
       <c r="AF24">
-        <v>1.79</v>
+        <v>2.09</v>
       </c>
       <c r="AG24">
         <v>0.17</v>
       </c>
       <c r="AI24">
-        <v>2.2200000000000002</v>
+        <v>2.52</v>
       </c>
       <c r="AJ24">
         <v>0.28000000000000003</v>
       </c>
       <c r="AL24">
-        <v>2.73</v>
+        <v>3.03</v>
       </c>
       <c r="AM24">
         <v>0.19</v>
@@ -13666,13 +13795,13 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="AF25">
-        <v>1.82</v>
+        <v>2.12</v>
       </c>
       <c r="AG25">
         <v>0.2</v>
       </c>
       <c r="AL25">
-        <v>2.74</v>
+        <v>3.04</v>
       </c>
       <c r="AM25">
         <v>0.2</v>
@@ -13720,13 +13849,13 @@
         <v>2.7039900000000001</v>
       </c>
       <c r="AF26">
-        <v>1.84</v>
+        <v>2.14</v>
       </c>
       <c r="AG26">
         <v>0.22</v>
       </c>
       <c r="AL26">
-        <v>2.77</v>
+        <v>3.07</v>
       </c>
       <c r="AM26">
         <v>0.22</v>
@@ -13774,13 +13903,13 @@
         <v>2.8181700000000003</v>
       </c>
       <c r="AF27">
-        <v>1.86</v>
+        <v>2.16</v>
       </c>
       <c r="AG27">
         <v>0.24</v>
       </c>
       <c r="AL27">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="AM27">
         <v>0.24</v>
@@ -13828,13 +13957,13 @@
         <v>2.9907899999999996</v>
       </c>
       <c r="AF28">
-        <v>1.88</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="AG28">
         <v>0.26</v>
       </c>
       <c r="AL28">
-        <v>2.83</v>
+        <v>3.13</v>
       </c>
       <c r="AM28">
         <v>0.26</v>
@@ -13872,13 +14001,13 @@
         <v>3.0956999999999999</v>
       </c>
       <c r="AF29">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AG29">
         <v>0.28000000000000003</v>
       </c>
       <c r="AL29">
-        <v>2.85</v>
+        <v>3.15</v>
       </c>
       <c r="AM29">
         <v>0.28000000000000003</v>

</xml_diff>